<commit_message>
web scrapping em novos sites
</commit_message>
<xml_diff>
--- a/remax_imoveis.xlsx
+++ b/remax_imoveis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,41 +444,6 @@
           <t>Link</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Preço</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo Imóvel</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Área</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quartos</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Banheiros</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Ambientes Totais</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>